<commit_message>
saved accuracy graph as pdf and got the excel file back
</commit_message>
<xml_diff>
--- a/rnn/acc_loss_graph_data.xlsx
+++ b/rnn/acc_loss_graph_data.xlsx
@@ -95,6 +95,3107 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Loss</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>training loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.6589</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4429</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4213</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3961</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3776</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3828</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3641</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.333</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.337</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.3242</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.3162</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.3041</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.3059</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3067</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.2874</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.3202</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.2869</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.2834</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.2846</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.2682</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.2622</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.2549</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.2451</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.2544</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.2365</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.2315</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.228</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.2575</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.2325</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.2406</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.2174</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.2082</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.2007</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.2033</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.198</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.1824</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.1763</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.1752</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.1765</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.1676</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.166</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.1781</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.2114</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.197</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.1753</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.1546</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.1543</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>validation loss </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.5259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5144</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.407</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4094</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5977</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4222</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3531</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3713</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3468</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.3369</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.3177</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.3424</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3177</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.3299</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.3051</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.3066</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.2994</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.2956</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.2951</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.274</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.2854</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.2812</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.2833</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.2719</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.2908</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.2714</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.2734</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.2907</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.2711</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.2534</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.271</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.2933</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.2641</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.2706</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.2745</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.2661</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.2678</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.2645</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.2742</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.2794</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.3036</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.3214</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.2628</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.2637</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.289</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.2924</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2069193456"/>
+        <c:axId val="-2090042288"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2069193456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2090042288"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2090042288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2069193456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Accuracy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>training accuracy </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.5925</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.772</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8171</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8288</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8404</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8398</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8478</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.862</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8623</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.8682</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.8724</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8775</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.8768</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.8746</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8864</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.8711</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.8865</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.8887</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.8869</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.8943</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.8983</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.9009</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.905</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.9025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.9096</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.9114</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.913</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.8997</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.9121</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.9098</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.9174</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.9175</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.9226</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.9251</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.9256</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9271</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.9331</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.9358</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.9357</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.9355</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.9381</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.9396</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.9335</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.9201</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.9245</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.9349</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.9436</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.9425</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>validation accuracy </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.7562</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7621</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7586</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7864</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7864</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8248</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7334</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8276</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8554</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8446</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8591</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.8642</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.8642</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8733</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.8572</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.8715</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8621</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.8757</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.8822</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.8776</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.8844</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.8861</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.8843</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.8946</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.892</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.8916</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.8916</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.8978</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.8881</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.8956</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.8952</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.8893</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.8967</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.9032</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.9029</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.8962</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.9003</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9018</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.8991</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.9056</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.9034</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.9046</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.9008</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.8977</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.8916</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.862</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.9011</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.9067</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.9005</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.9005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2071797520"/>
+        <c:axId val="-2089494352"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2071797520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2089494352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2089494352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2071797520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -362,8 +3463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1243,5 +4344,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>